<commit_message>
Fixed the same again
</commit_message>
<xml_diff>
--- a/gdp_revisions_datasets/base_year_dummies_df.xlsx
+++ b/gdp_revisions_datasets/base_year_dummies_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_9B376725C2595EDEE54878D6425DCE3A76D568BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40140D38-8F5E-4001-B068-4AA062F87748}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_965A6736C2595EDEE54878D6425DCE3A8654943E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9278EB4-9175-41D0-983F-357890384E61}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22782" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22117" uniqueCount="499">
   <si>
     <t>year</t>
   </si>
@@ -1889,14 +1889,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:OA1475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE314" workbookViewId="0">
-      <selection activeCell="CM328" sqref="CM328:DA334"/>
+    <sheetView tabSelected="1" topLeftCell="CH313" workbookViewId="0">
+      <selection activeCell="CL322" sqref="CL322:DA332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:391" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -19542,8 +19539,8 @@
       <c r="CM277" t="s">
         <v>414</v>
       </c>
-      <c r="CN277" t="s">
-        <v>415</v>
+      <c r="CN277">
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19604,8 +19601,8 @@
       <c r="CM278" t="s">
         <v>414</v>
       </c>
-      <c r="CN278" t="s">
-        <v>415</v>
+      <c r="CN278">
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19666,8 +19663,8 @@
       <c r="CM279" t="s">
         <v>414</v>
       </c>
-      <c r="CN279" t="s">
-        <v>415</v>
+      <c r="CN279">
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19728,8 +19725,8 @@
       <c r="CM280" t="s">
         <v>413</v>
       </c>
-      <c r="CN280" t="s">
-        <v>414</v>
+      <c r="CN280">
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19790,11 +19787,11 @@
       <c r="CM281" t="s">
         <v>413</v>
       </c>
-      <c r="CN281" t="s">
-        <v>414</v>
-      </c>
-      <c r="CO281" t="s">
-        <v>415</v>
+      <c r="CN281">
+        <v>0</v>
+      </c>
+      <c r="CO281">
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19855,11 +19852,11 @@
       <c r="CM282" t="s">
         <v>413</v>
       </c>
-      <c r="CN282" t="s">
-        <v>414</v>
-      </c>
-      <c r="CO282" t="s">
-        <v>415</v>
+      <c r="CN282">
+        <v>0</v>
+      </c>
+      <c r="CO282">
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19920,11 +19917,11 @@
       <c r="CM283" t="s">
         <v>413</v>
       </c>
-      <c r="CN283" t="s">
-        <v>414</v>
-      </c>
-      <c r="CO283" t="s">
-        <v>415</v>
+      <c r="CN283">
+        <v>0</v>
+      </c>
+      <c r="CO283">
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -19985,11 +19982,11 @@
       <c r="CM284" t="s">
         <v>412</v>
       </c>
-      <c r="CN284" t="s">
-        <v>413</v>
-      </c>
-      <c r="CO284" t="s">
-        <v>414</v>
+      <c r="CN284">
+        <v>0</v>
+      </c>
+      <c r="CO284">
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -20032,14 +20029,14 @@
       <c r="CM285" t="s">
         <v>412</v>
       </c>
-      <c r="CN285" t="s">
-        <v>413</v>
-      </c>
-      <c r="CO285" t="s">
-        <v>414</v>
-      </c>
-      <c r="CP285" t="s">
-        <v>415</v>
+      <c r="CN285">
+        <v>0</v>
+      </c>
+      <c r="CO285">
+        <v>0</v>
+      </c>
+      <c r="CP285">
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -20082,14 +20079,14 @@
       <c r="CM286" t="s">
         <v>412</v>
       </c>
-      <c r="CN286" t="s">
-        <v>413</v>
-      </c>
-      <c r="CO286" t="s">
-        <v>414</v>
-      </c>
-      <c r="CP286" t="s">
-        <v>415</v>
+      <c r="CN286">
+        <v>0</v>
+      </c>
+      <c r="CO286">
+        <v>0</v>
+      </c>
+      <c r="CP286">
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -20132,14 +20129,14 @@
       <c r="CM287" t="s">
         <v>412</v>
       </c>
-      <c r="CN287" t="s">
-        <v>413</v>
-      </c>
-      <c r="CO287" t="s">
-        <v>414</v>
-      </c>
-      <c r="CP287" t="s">
-        <v>415</v>
+      <c r="CN287">
+        <v>0</v>
+      </c>
+      <c r="CO287">
+        <v>0</v>
+      </c>
+      <c r="CP287">
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:94" hidden="1" x14ac:dyDescent="0.3">
@@ -20182,14 +20179,14 @@
       <c r="CM288" t="s">
         <v>411</v>
       </c>
-      <c r="CN288" t="s">
-        <v>412</v>
-      </c>
-      <c r="CO288" t="s">
-        <v>413</v>
-      </c>
-      <c r="CP288" t="s">
-        <v>414</v>
+      <c r="CN288">
+        <v>0</v>
+      </c>
+      <c r="CO288">
+        <v>0</v>
+      </c>
+      <c r="CP288">
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20232,14 +20229,14 @@
       <c r="CM289" t="s">
         <v>411</v>
       </c>
-      <c r="CN289" t="s">
-        <v>412</v>
-      </c>
-      <c r="CO289" t="s">
-        <v>413</v>
-      </c>
-      <c r="CP289" t="s">
-        <v>414</v>
+      <c r="CN289">
+        <v>0</v>
+      </c>
+      <c r="CO289">
+        <v>0</v>
+      </c>
+      <c r="CP289">
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20279,17 +20276,17 @@
       <c r="CM290" t="s">
         <v>411</v>
       </c>
-      <c r="CN290" t="s">
-        <v>412</v>
-      </c>
-      <c r="CO290" t="s">
-        <v>413</v>
-      </c>
-      <c r="CP290" t="s">
-        <v>414</v>
-      </c>
-      <c r="CQ290" t="s">
-        <v>415</v>
+      <c r="CN290">
+        <v>0</v>
+      </c>
+      <c r="CO290">
+        <v>0</v>
+      </c>
+      <c r="CP290">
+        <v>0</v>
+      </c>
+      <c r="CQ290">
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20329,17 +20326,17 @@
       <c r="CM291" t="s">
         <v>411</v>
       </c>
-      <c r="CN291" t="s">
-        <v>412</v>
-      </c>
-      <c r="CO291" t="s">
-        <v>413</v>
-      </c>
-      <c r="CP291" t="s">
-        <v>414</v>
-      </c>
-      <c r="CQ291" t="s">
-        <v>415</v>
+      <c r="CN291">
+        <v>0</v>
+      </c>
+      <c r="CO291">
+        <v>0</v>
+      </c>
+      <c r="CP291">
+        <v>0</v>
+      </c>
+      <c r="CQ291">
+        <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20379,17 +20376,17 @@
       <c r="CM292" t="s">
         <v>411</v>
       </c>
-      <c r="CN292" t="s">
-        <v>412</v>
-      </c>
-      <c r="CO292" t="s">
-        <v>413</v>
-      </c>
-      <c r="CP292" t="s">
-        <v>414</v>
-      </c>
-      <c r="CQ292" t="s">
-        <v>415</v>
+      <c r="CN292">
+        <v>0</v>
+      </c>
+      <c r="CO292">
+        <v>0</v>
+      </c>
+      <c r="CP292">
+        <v>0</v>
+      </c>
+      <c r="CQ292">
+        <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20429,17 +20426,17 @@
       <c r="CM293" t="s">
         <v>410</v>
       </c>
-      <c r="CN293" t="s">
-        <v>411</v>
-      </c>
-      <c r="CO293" t="s">
-        <v>412</v>
-      </c>
-      <c r="CP293" t="s">
-        <v>413</v>
-      </c>
-      <c r="CQ293" t="s">
-        <v>414</v>
+      <c r="CN293">
+        <v>0</v>
+      </c>
+      <c r="CO293">
+        <v>0</v>
+      </c>
+      <c r="CP293">
+        <v>0</v>
+      </c>
+      <c r="CQ293">
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20476,20 +20473,20 @@
       <c r="CM294" t="s">
         <v>410</v>
       </c>
-      <c r="CN294" t="s">
-        <v>411</v>
-      </c>
-      <c r="CO294" t="s">
-        <v>412</v>
-      </c>
-      <c r="CP294" t="s">
-        <v>413</v>
-      </c>
-      <c r="CQ294" t="s">
-        <v>414</v>
-      </c>
-      <c r="CR294" t="s">
-        <v>415</v>
+      <c r="CN294">
+        <v>0</v>
+      </c>
+      <c r="CO294">
+        <v>0</v>
+      </c>
+      <c r="CP294">
+        <v>0</v>
+      </c>
+      <c r="CQ294">
+        <v>0</v>
+      </c>
+      <c r="CR294">
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20526,20 +20523,20 @@
       <c r="CM295" t="s">
         <v>410</v>
       </c>
-      <c r="CN295" t="s">
-        <v>411</v>
-      </c>
-      <c r="CO295" t="s">
-        <v>412</v>
-      </c>
-      <c r="CP295" t="s">
-        <v>413</v>
-      </c>
-      <c r="CQ295" t="s">
-        <v>414</v>
-      </c>
-      <c r="CR295" t="s">
-        <v>415</v>
+      <c r="CN295">
+        <v>0</v>
+      </c>
+      <c r="CO295">
+        <v>0</v>
+      </c>
+      <c r="CP295">
+        <v>0</v>
+      </c>
+      <c r="CQ295">
+        <v>0</v>
+      </c>
+      <c r="CR295">
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20576,20 +20573,20 @@
       <c r="CM296" t="s">
         <v>410</v>
       </c>
-      <c r="CN296" t="s">
-        <v>411</v>
-      </c>
-      <c r="CO296" t="s">
-        <v>412</v>
-      </c>
-      <c r="CP296" t="s">
-        <v>413</v>
-      </c>
-      <c r="CQ296" t="s">
-        <v>414</v>
-      </c>
-      <c r="CR296" t="s">
-        <v>415</v>
+      <c r="CN296">
+        <v>0</v>
+      </c>
+      <c r="CO296">
+        <v>0</v>
+      </c>
+      <c r="CP296">
+        <v>0</v>
+      </c>
+      <c r="CQ296">
+        <v>0</v>
+      </c>
+      <c r="CR296">
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20626,20 +20623,20 @@
       <c r="CM297" t="s">
         <v>409</v>
       </c>
-      <c r="CN297" t="s">
-        <v>410</v>
-      </c>
-      <c r="CO297" t="s">
-        <v>411</v>
-      </c>
-      <c r="CP297" t="s">
-        <v>412</v>
-      </c>
-      <c r="CQ297" t="s">
-        <v>413</v>
-      </c>
-      <c r="CR297" t="s">
-        <v>414</v>
+      <c r="CN297">
+        <v>0</v>
+      </c>
+      <c r="CO297">
+        <v>0</v>
+      </c>
+      <c r="CP297">
+        <v>0</v>
+      </c>
+      <c r="CQ297">
+        <v>0</v>
+      </c>
+      <c r="CR297">
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20676,20 +20673,20 @@
       <c r="CM298" t="s">
         <v>409</v>
       </c>
-      <c r="CN298" t="s">
-        <v>410</v>
-      </c>
-      <c r="CO298" t="s">
-        <v>411</v>
-      </c>
-      <c r="CP298" t="s">
-        <v>412</v>
-      </c>
-      <c r="CQ298" t="s">
-        <v>413</v>
-      </c>
-      <c r="CR298" t="s">
-        <v>414</v>
+      <c r="CN298">
+        <v>0</v>
+      </c>
+      <c r="CO298">
+        <v>0</v>
+      </c>
+      <c r="CP298">
+        <v>0</v>
+      </c>
+      <c r="CQ298">
+        <v>0</v>
+      </c>
+      <c r="CR298">
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20723,23 +20720,23 @@
       <c r="CM299" t="s">
         <v>409</v>
       </c>
-      <c r="CN299" t="s">
-        <v>410</v>
-      </c>
-      <c r="CO299" t="s">
-        <v>411</v>
-      </c>
-      <c r="CP299" t="s">
-        <v>412</v>
-      </c>
-      <c r="CQ299" t="s">
-        <v>413</v>
-      </c>
-      <c r="CR299" t="s">
-        <v>414</v>
-      </c>
-      <c r="CS299" t="s">
-        <v>415</v>
+      <c r="CN299">
+        <v>0</v>
+      </c>
+      <c r="CO299">
+        <v>0</v>
+      </c>
+      <c r="CP299">
+        <v>0</v>
+      </c>
+      <c r="CQ299">
+        <v>0</v>
+      </c>
+      <c r="CR299">
+        <v>0</v>
+      </c>
+      <c r="CS299">
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20773,23 +20770,23 @@
       <c r="CM300" t="s">
         <v>409</v>
       </c>
-      <c r="CN300" t="s">
-        <v>410</v>
-      </c>
-      <c r="CO300" t="s">
-        <v>411</v>
-      </c>
-      <c r="CP300" t="s">
-        <v>412</v>
-      </c>
-      <c r="CQ300" t="s">
-        <v>413</v>
-      </c>
-      <c r="CR300" t="s">
-        <v>414</v>
-      </c>
-      <c r="CS300" t="s">
-        <v>415</v>
+      <c r="CN300">
+        <v>0</v>
+      </c>
+      <c r="CO300">
+        <v>0</v>
+      </c>
+      <c r="CP300">
+        <v>0</v>
+      </c>
+      <c r="CQ300">
+        <v>0</v>
+      </c>
+      <c r="CR300">
+        <v>0</v>
+      </c>
+      <c r="CS300">
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:98" hidden="1" x14ac:dyDescent="0.3">
@@ -20823,23 +20820,23 @@
       <c r="CM301" t="s">
         <v>409</v>
       </c>
-      <c r="CN301" t="s">
-        <v>410</v>
-      </c>
-      <c r="CO301" t="s">
-        <v>411</v>
-      </c>
-      <c r="CP301" t="s">
-        <v>412</v>
-      </c>
-      <c r="CQ301" t="s">
-        <v>413</v>
-      </c>
-      <c r="CR301" t="s">
-        <v>414</v>
-      </c>
-      <c r="CS301" t="s">
-        <v>415</v>
+      <c r="CN301">
+        <v>0</v>
+      </c>
+      <c r="CO301">
+        <v>0</v>
+      </c>
+      <c r="CP301">
+        <v>0</v>
+      </c>
+      <c r="CQ301">
+        <v>0</v>
+      </c>
+      <c r="CR301">
+        <v>0</v>
+      </c>
+      <c r="CS301">
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:98" x14ac:dyDescent="0.3">
@@ -20873,23 +20870,23 @@
       <c r="CM302" t="s">
         <v>408</v>
       </c>
-      <c r="CN302" t="s">
-        <v>409</v>
-      </c>
-      <c r="CO302" t="s">
-        <v>410</v>
-      </c>
-      <c r="CP302" t="s">
-        <v>411</v>
-      </c>
-      <c r="CQ302" t="s">
-        <v>412</v>
-      </c>
-      <c r="CR302" t="s">
-        <v>413</v>
-      </c>
-      <c r="CS302" t="s">
-        <v>414</v>
+      <c r="CN302">
+        <v>0</v>
+      </c>
+      <c r="CO302">
+        <v>0</v>
+      </c>
+      <c r="CP302">
+        <v>0</v>
+      </c>
+      <c r="CQ302">
+        <v>0</v>
+      </c>
+      <c r="CR302">
+        <v>0</v>
+      </c>
+      <c r="CS302">
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:98" x14ac:dyDescent="0.3">
@@ -20920,26 +20917,26 @@
       <c r="CM303" t="s">
         <v>408</v>
       </c>
-      <c r="CN303" t="s">
-        <v>409</v>
-      </c>
-      <c r="CO303" t="s">
-        <v>410</v>
-      </c>
-      <c r="CP303" t="s">
-        <v>411</v>
-      </c>
-      <c r="CQ303" t="s">
-        <v>412</v>
-      </c>
-      <c r="CR303" t="s">
-        <v>413</v>
-      </c>
-      <c r="CS303" t="s">
-        <v>414</v>
-      </c>
-      <c r="CT303" t="s">
-        <v>415</v>
+      <c r="CN303">
+        <v>0</v>
+      </c>
+      <c r="CO303">
+        <v>0</v>
+      </c>
+      <c r="CP303">
+        <v>0</v>
+      </c>
+      <c r="CQ303">
+        <v>0</v>
+      </c>
+      <c r="CR303">
+        <v>0</v>
+      </c>
+      <c r="CS303">
+        <v>0</v>
+      </c>
+      <c r="CT303">
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:98" x14ac:dyDescent="0.3">
@@ -20970,26 +20967,26 @@
       <c r="CM304" t="s">
         <v>408</v>
       </c>
-      <c r="CN304" t="s">
-        <v>409</v>
-      </c>
-      <c r="CO304" t="s">
-        <v>410</v>
-      </c>
-      <c r="CP304" t="s">
-        <v>411</v>
-      </c>
-      <c r="CQ304" t="s">
-        <v>412</v>
-      </c>
-      <c r="CR304" t="s">
-        <v>413</v>
-      </c>
-      <c r="CS304" t="s">
-        <v>414</v>
-      </c>
-      <c r="CT304" t="s">
-        <v>415</v>
+      <c r="CN304">
+        <v>0</v>
+      </c>
+      <c r="CO304">
+        <v>0</v>
+      </c>
+      <c r="CP304">
+        <v>0</v>
+      </c>
+      <c r="CQ304">
+        <v>0</v>
+      </c>
+      <c r="CR304">
+        <v>0</v>
+      </c>
+      <c r="CS304">
+        <v>0</v>
+      </c>
+      <c r="CT304">
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:102" x14ac:dyDescent="0.3">
@@ -21020,26 +21017,26 @@
       <c r="CM305" t="s">
         <v>408</v>
       </c>
-      <c r="CN305" t="s">
-        <v>409</v>
-      </c>
-      <c r="CO305" t="s">
-        <v>410</v>
-      </c>
-      <c r="CP305" t="s">
-        <v>411</v>
-      </c>
-      <c r="CQ305" t="s">
-        <v>412</v>
-      </c>
-      <c r="CR305" t="s">
-        <v>413</v>
-      </c>
-      <c r="CS305" t="s">
-        <v>414</v>
-      </c>
-      <c r="CT305" t="s">
-        <v>415</v>
+      <c r="CN305">
+        <v>0</v>
+      </c>
+      <c r="CO305">
+        <v>0</v>
+      </c>
+      <c r="CP305">
+        <v>0</v>
+      </c>
+      <c r="CQ305">
+        <v>0</v>
+      </c>
+      <c r="CR305">
+        <v>0</v>
+      </c>
+      <c r="CS305">
+        <v>0</v>
+      </c>
+      <c r="CT305">
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:102" x14ac:dyDescent="0.3">
@@ -21070,26 +21067,26 @@
       <c r="CM306" t="s">
         <v>407</v>
       </c>
-      <c r="CN306" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO306" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP306" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ306" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR306" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS306" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT306" t="s">
-        <v>414</v>
+      <c r="CN306">
+        <v>0</v>
+      </c>
+      <c r="CO306">
+        <v>0</v>
+      </c>
+      <c r="CP306">
+        <v>0</v>
+      </c>
+      <c r="CQ306">
+        <v>0</v>
+      </c>
+      <c r="CR306">
+        <v>0</v>
+      </c>
+      <c r="CS306">
+        <v>0</v>
+      </c>
+      <c r="CT306">
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:102" x14ac:dyDescent="0.3">
@@ -21117,29 +21114,29 @@
       <c r="CM307" t="s">
         <v>407</v>
       </c>
-      <c r="CN307" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO307" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP307" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ307" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR307" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS307" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT307" t="s">
-        <v>414</v>
-      </c>
-      <c r="CU307" t="s">
-        <v>415</v>
+      <c r="CN307">
+        <v>0</v>
+      </c>
+      <c r="CO307">
+        <v>0</v>
+      </c>
+      <c r="CP307">
+        <v>0</v>
+      </c>
+      <c r="CQ307">
+        <v>0</v>
+      </c>
+      <c r="CR307">
+        <v>0</v>
+      </c>
+      <c r="CS307">
+        <v>0</v>
+      </c>
+      <c r="CT307">
+        <v>0</v>
+      </c>
+      <c r="CU307">
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:102" x14ac:dyDescent="0.3">
@@ -21167,29 +21164,29 @@
       <c r="CM308" t="s">
         <v>407</v>
       </c>
-      <c r="CN308" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO308" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP308" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ308" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR308" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS308" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT308" t="s">
-        <v>414</v>
-      </c>
-      <c r="CU308" t="s">
-        <v>415</v>
+      <c r="CN308">
+        <v>0</v>
+      </c>
+      <c r="CO308">
+        <v>0</v>
+      </c>
+      <c r="CP308">
+        <v>0</v>
+      </c>
+      <c r="CQ308">
+        <v>0</v>
+      </c>
+      <c r="CR308">
+        <v>0</v>
+      </c>
+      <c r="CS308">
+        <v>0</v>
+      </c>
+      <c r="CT308">
+        <v>0</v>
+      </c>
+      <c r="CU308">
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:102" x14ac:dyDescent="0.3">
@@ -21217,29 +21214,29 @@
       <c r="CM309" t="s">
         <v>407</v>
       </c>
-      <c r="CN309" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO309" t="s">
-        <v>409</v>
-      </c>
-      <c r="CP309" t="s">
-        <v>410</v>
-      </c>
-      <c r="CQ309" t="s">
-        <v>411</v>
-      </c>
-      <c r="CR309" t="s">
-        <v>412</v>
-      </c>
-      <c r="CS309" t="s">
-        <v>413</v>
-      </c>
-      <c r="CT309" t="s">
-        <v>414</v>
-      </c>
-      <c r="CU309" t="s">
-        <v>415</v>
+      <c r="CN309">
+        <v>0</v>
+      </c>
+      <c r="CO309">
+        <v>0</v>
+      </c>
+      <c r="CP309">
+        <v>0</v>
+      </c>
+      <c r="CQ309">
+        <v>0</v>
+      </c>
+      <c r="CR309">
+        <v>0</v>
+      </c>
+      <c r="CS309">
+        <v>0</v>
+      </c>
+      <c r="CT309">
+        <v>0</v>
+      </c>
+      <c r="CU309">
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:102" x14ac:dyDescent="0.3">
@@ -21267,29 +21264,29 @@
       <c r="CM310" t="s">
         <v>406</v>
       </c>
-      <c r="CN310" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO310" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP310" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ310" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR310" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS310" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT310" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU310" t="s">
-        <v>414</v>
+      <c r="CN310">
+        <v>0</v>
+      </c>
+      <c r="CO310">
+        <v>0</v>
+      </c>
+      <c r="CP310">
+        <v>0</v>
+      </c>
+      <c r="CQ310">
+        <v>0</v>
+      </c>
+      <c r="CR310">
+        <v>0</v>
+      </c>
+      <c r="CS310">
+        <v>0</v>
+      </c>
+      <c r="CT310">
+        <v>0</v>
+      </c>
+      <c r="CU310">
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:102" x14ac:dyDescent="0.3">
@@ -21314,32 +21311,32 @@
       <c r="CM311" t="s">
         <v>406</v>
       </c>
-      <c r="CN311" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO311" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP311" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ311" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR311" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS311" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT311" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU311" t="s">
-        <v>414</v>
-      </c>
-      <c r="CV311" t="s">
-        <v>415</v>
+      <c r="CN311">
+        <v>0</v>
+      </c>
+      <c r="CO311">
+        <v>0</v>
+      </c>
+      <c r="CP311">
+        <v>0</v>
+      </c>
+      <c r="CQ311">
+        <v>0</v>
+      </c>
+      <c r="CR311">
+        <v>0</v>
+      </c>
+      <c r="CS311">
+        <v>0</v>
+      </c>
+      <c r="CT311">
+        <v>0</v>
+      </c>
+      <c r="CU311">
+        <v>0</v>
+      </c>
+      <c r="CV311">
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:102" x14ac:dyDescent="0.3">
@@ -21364,32 +21361,32 @@
       <c r="CM312" t="s">
         <v>406</v>
       </c>
-      <c r="CN312" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO312" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP312" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ312" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR312" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS312" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT312" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU312" t="s">
-        <v>414</v>
-      </c>
-      <c r="CV312" t="s">
-        <v>415</v>
+      <c r="CN312">
+        <v>0</v>
+      </c>
+      <c r="CO312">
+        <v>0</v>
+      </c>
+      <c r="CP312">
+        <v>0</v>
+      </c>
+      <c r="CQ312">
+        <v>0</v>
+      </c>
+      <c r="CR312">
+        <v>0</v>
+      </c>
+      <c r="CS312">
+        <v>0</v>
+      </c>
+      <c r="CT312">
+        <v>0</v>
+      </c>
+      <c r="CU312">
+        <v>0</v>
+      </c>
+      <c r="CV312">
+        <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:102" x14ac:dyDescent="0.3">
@@ -21414,32 +21411,32 @@
       <c r="CM313" t="s">
         <v>406</v>
       </c>
-      <c r="CN313" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO313" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP313" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ313" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR313" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS313" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT313" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU313" t="s">
-        <v>414</v>
-      </c>
-      <c r="CV313" t="s">
-        <v>415</v>
+      <c r="CN313">
+        <v>0</v>
+      </c>
+      <c r="CO313">
+        <v>0</v>
+      </c>
+      <c r="CP313">
+        <v>0</v>
+      </c>
+      <c r="CQ313">
+        <v>0</v>
+      </c>
+      <c r="CR313">
+        <v>0</v>
+      </c>
+      <c r="CS313">
+        <v>0</v>
+      </c>
+      <c r="CT313">
+        <v>0</v>
+      </c>
+      <c r="CU313">
+        <v>0</v>
+      </c>
+      <c r="CV313">
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:102" x14ac:dyDescent="0.3">
@@ -21464,32 +21461,32 @@
       <c r="CM314" t="s">
         <v>406</v>
       </c>
-      <c r="CN314" t="s">
-        <v>407</v>
-      </c>
-      <c r="CO314" t="s">
-        <v>408</v>
-      </c>
-      <c r="CP314" t="s">
-        <v>409</v>
-      </c>
-      <c r="CQ314" t="s">
-        <v>410</v>
-      </c>
-      <c r="CR314" t="s">
-        <v>411</v>
-      </c>
-      <c r="CS314" t="s">
-        <v>412</v>
-      </c>
-      <c r="CT314" t="s">
-        <v>413</v>
-      </c>
-      <c r="CU314" t="s">
-        <v>414</v>
-      </c>
-      <c r="CV314" t="s">
-        <v>415</v>
+      <c r="CN314">
+        <v>0</v>
+      </c>
+      <c r="CO314">
+        <v>0</v>
+      </c>
+      <c r="CP314">
+        <v>0</v>
+      </c>
+      <c r="CQ314">
+        <v>0</v>
+      </c>
+      <c r="CR314">
+        <v>0</v>
+      </c>
+      <c r="CS314">
+        <v>0</v>
+      </c>
+      <c r="CT314">
+        <v>0</v>
+      </c>
+      <c r="CU314">
+        <v>0</v>
+      </c>
+      <c r="CV314">
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:102" x14ac:dyDescent="0.3">
@@ -21511,35 +21508,35 @@
       <c r="CM315" t="s">
         <v>405</v>
       </c>
-      <c r="CN315" t="s">
-        <v>406</v>
-      </c>
-      <c r="CO315" t="s">
-        <v>407</v>
-      </c>
-      <c r="CP315" t="s">
-        <v>408</v>
-      </c>
-      <c r="CQ315" t="s">
-        <v>409</v>
-      </c>
-      <c r="CR315" t="s">
-        <v>410</v>
-      </c>
-      <c r="CS315" t="s">
-        <v>411</v>
-      </c>
-      <c r="CT315" t="s">
-        <v>412</v>
-      </c>
-      <c r="CU315" t="s">
-        <v>413</v>
-      </c>
-      <c r="CV315" t="s">
-        <v>414</v>
-      </c>
-      <c r="CW315" t="s">
-        <v>415</v>
+      <c r="CN315">
+        <v>0</v>
+      </c>
+      <c r="CO315">
+        <v>0</v>
+      </c>
+      <c r="CP315">
+        <v>0</v>
+      </c>
+      <c r="CQ315">
+        <v>0</v>
+      </c>
+      <c r="CR315">
+        <v>0</v>
+      </c>
+      <c r="CS315">
+        <v>0</v>
+      </c>
+      <c r="CT315">
+        <v>0</v>
+      </c>
+      <c r="CU315">
+        <v>0</v>
+      </c>
+      <c r="CV315">
+        <v>0</v>
+      </c>
+      <c r="CW315">
+        <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:102" x14ac:dyDescent="0.3">
@@ -21561,35 +21558,35 @@
       <c r="CM316" t="s">
         <v>405</v>
       </c>
-      <c r="CN316" t="s">
-        <v>406</v>
-      </c>
-      <c r="CO316" t="s">
-        <v>407</v>
-      </c>
-      <c r="CP316" t="s">
-        <v>408</v>
-      </c>
-      <c r="CQ316" t="s">
-        <v>409</v>
-      </c>
-      <c r="CR316" t="s">
-        <v>410</v>
-      </c>
-      <c r="CS316" t="s">
-        <v>411</v>
-      </c>
-      <c r="CT316" t="s">
-        <v>412</v>
-      </c>
-      <c r="CU316" t="s">
-        <v>413</v>
-      </c>
-      <c r="CV316" t="s">
-        <v>414</v>
-      </c>
-      <c r="CW316" t="s">
-        <v>415</v>
+      <c r="CN316">
+        <v>0</v>
+      </c>
+      <c r="CO316">
+        <v>0</v>
+      </c>
+      <c r="CP316">
+        <v>0</v>
+      </c>
+      <c r="CQ316">
+        <v>0</v>
+      </c>
+      <c r="CR316">
+        <v>0</v>
+      </c>
+      <c r="CS316">
+        <v>0</v>
+      </c>
+      <c r="CT316">
+        <v>0</v>
+      </c>
+      <c r="CU316">
+        <v>0</v>
+      </c>
+      <c r="CV316">
+        <v>0</v>
+      </c>
+      <c r="CW316">
+        <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:102" x14ac:dyDescent="0.3">
@@ -21611,35 +21608,35 @@
       <c r="CM317" t="s">
         <v>405</v>
       </c>
-      <c r="CN317" t="s">
-        <v>406</v>
-      </c>
-      <c r="CO317" t="s">
-        <v>407</v>
-      </c>
-      <c r="CP317" t="s">
-        <v>408</v>
-      </c>
-      <c r="CQ317" t="s">
-        <v>409</v>
-      </c>
-      <c r="CR317" t="s">
-        <v>410</v>
-      </c>
-      <c r="CS317" t="s">
-        <v>411</v>
-      </c>
-      <c r="CT317" t="s">
-        <v>412</v>
-      </c>
-      <c r="CU317" t="s">
-        <v>413</v>
-      </c>
-      <c r="CV317" t="s">
-        <v>414</v>
-      </c>
-      <c r="CW317" t="s">
-        <v>415</v>
+      <c r="CN317">
+        <v>0</v>
+      </c>
+      <c r="CO317">
+        <v>0</v>
+      </c>
+      <c r="CP317">
+        <v>0</v>
+      </c>
+      <c r="CQ317">
+        <v>0</v>
+      </c>
+      <c r="CR317">
+        <v>0</v>
+      </c>
+      <c r="CS317">
+        <v>0</v>
+      </c>
+      <c r="CT317">
+        <v>0</v>
+      </c>
+      <c r="CU317">
+        <v>0</v>
+      </c>
+      <c r="CV317">
+        <v>0</v>
+      </c>
+      <c r="CW317">
+        <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:102" x14ac:dyDescent="0.3">
@@ -21661,35 +21658,35 @@
       <c r="CM318" t="s">
         <v>404</v>
       </c>
-      <c r="CN318" t="s">
-        <v>405</v>
-      </c>
-      <c r="CO318" t="s">
-        <v>406</v>
-      </c>
-      <c r="CP318" t="s">
-        <v>407</v>
-      </c>
-      <c r="CQ318" t="s">
-        <v>408</v>
-      </c>
-      <c r="CR318" t="s">
-        <v>409</v>
-      </c>
-      <c r="CS318" t="s">
-        <v>410</v>
-      </c>
-      <c r="CT318" t="s">
-        <v>411</v>
-      </c>
-      <c r="CU318" t="s">
-        <v>412</v>
-      </c>
-      <c r="CV318" t="s">
-        <v>413</v>
-      </c>
-      <c r="CW318" t="s">
-        <v>414</v>
+      <c r="CN318">
+        <v>0</v>
+      </c>
+      <c r="CO318">
+        <v>0</v>
+      </c>
+      <c r="CP318">
+        <v>0</v>
+      </c>
+      <c r="CQ318">
+        <v>0</v>
+      </c>
+      <c r="CR318">
+        <v>0</v>
+      </c>
+      <c r="CS318">
+        <v>0</v>
+      </c>
+      <c r="CT318">
+        <v>0</v>
+      </c>
+      <c r="CU318">
+        <v>0</v>
+      </c>
+      <c r="CV318">
+        <v>0</v>
+      </c>
+      <c r="CW318">
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:102" x14ac:dyDescent="0.3">
@@ -21708,38 +21705,38 @@
       <c r="CM319" t="s">
         <v>404</v>
       </c>
-      <c r="CN319" t="s">
-        <v>405</v>
-      </c>
-      <c r="CO319" t="s">
-        <v>406</v>
-      </c>
-      <c r="CP319" t="s">
-        <v>407</v>
-      </c>
-      <c r="CQ319" t="s">
-        <v>408</v>
-      </c>
-      <c r="CR319" t="s">
-        <v>409</v>
-      </c>
-      <c r="CS319" t="s">
-        <v>410</v>
-      </c>
-      <c r="CT319" t="s">
-        <v>411</v>
-      </c>
-      <c r="CU319" t="s">
-        <v>412</v>
-      </c>
-      <c r="CV319" t="s">
-        <v>413</v>
-      </c>
-      <c r="CW319" t="s">
-        <v>414</v>
-      </c>
-      <c r="CX319" t="s">
-        <v>415</v>
+      <c r="CN319">
+        <v>0</v>
+      </c>
+      <c r="CO319">
+        <v>0</v>
+      </c>
+      <c r="CP319">
+        <v>0</v>
+      </c>
+      <c r="CQ319">
+        <v>0</v>
+      </c>
+      <c r="CR319">
+        <v>0</v>
+      </c>
+      <c r="CS319">
+        <v>0</v>
+      </c>
+      <c r="CT319">
+        <v>0</v>
+      </c>
+      <c r="CU319">
+        <v>0</v>
+      </c>
+      <c r="CV319">
+        <v>0</v>
+      </c>
+      <c r="CW319">
+        <v>0</v>
+      </c>
+      <c r="CX319">
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:102" x14ac:dyDescent="0.3">
@@ -21758,38 +21755,38 @@
       <c r="CM320" t="s">
         <v>404</v>
       </c>
-      <c r="CN320" t="s">
-        <v>405</v>
-      </c>
-      <c r="CO320" t="s">
-        <v>406</v>
-      </c>
-      <c r="CP320" t="s">
-        <v>407</v>
-      </c>
-      <c r="CQ320" t="s">
-        <v>408</v>
-      </c>
-      <c r="CR320" t="s">
-        <v>409</v>
-      </c>
-      <c r="CS320" t="s">
-        <v>410</v>
-      </c>
-      <c r="CT320" t="s">
-        <v>411</v>
-      </c>
-      <c r="CU320" t="s">
-        <v>412</v>
-      </c>
-      <c r="CV320" t="s">
-        <v>413</v>
-      </c>
-      <c r="CW320" t="s">
-        <v>414</v>
-      </c>
-      <c r="CX320" t="s">
-        <v>415</v>
+      <c r="CN320">
+        <v>0</v>
+      </c>
+      <c r="CO320">
+        <v>0</v>
+      </c>
+      <c r="CP320">
+        <v>0</v>
+      </c>
+      <c r="CQ320">
+        <v>0</v>
+      </c>
+      <c r="CR320">
+        <v>0</v>
+      </c>
+      <c r="CS320">
+        <v>0</v>
+      </c>
+      <c r="CT320">
+        <v>0</v>
+      </c>
+      <c r="CU320">
+        <v>0</v>
+      </c>
+      <c r="CV320">
+        <v>0</v>
+      </c>
+      <c r="CW320">
+        <v>0</v>
+      </c>
+      <c r="CX320">
+        <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:106" x14ac:dyDescent="0.3">
@@ -21808,38 +21805,38 @@
       <c r="CM321" t="s">
         <v>404</v>
       </c>
-      <c r="CN321" t="s">
-        <v>405</v>
-      </c>
-      <c r="CO321" t="s">
-        <v>406</v>
-      </c>
-      <c r="CP321" t="s">
-        <v>407</v>
-      </c>
-      <c r="CQ321" t="s">
-        <v>408</v>
-      </c>
-      <c r="CR321" t="s">
-        <v>409</v>
-      </c>
-      <c r="CS321" t="s">
-        <v>410</v>
-      </c>
-      <c r="CT321" t="s">
-        <v>411</v>
-      </c>
-      <c r="CU321" t="s">
-        <v>412</v>
-      </c>
-      <c r="CV321" t="s">
-        <v>413</v>
-      </c>
-      <c r="CW321" t="s">
-        <v>414</v>
-      </c>
-      <c r="CX321" t="s">
-        <v>415</v>
+      <c r="CN321">
+        <v>0</v>
+      </c>
+      <c r="CO321">
+        <v>0</v>
+      </c>
+      <c r="CP321">
+        <v>0</v>
+      </c>
+      <c r="CQ321">
+        <v>0</v>
+      </c>
+      <c r="CR321">
+        <v>0</v>
+      </c>
+      <c r="CS321">
+        <v>0</v>
+      </c>
+      <c r="CT321">
+        <v>0</v>
+      </c>
+      <c r="CU321">
+        <v>0</v>
+      </c>
+      <c r="CV321">
+        <v>0</v>
+      </c>
+      <c r="CW321">
+        <v>0</v>
+      </c>
+      <c r="CX321">
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:106" x14ac:dyDescent="0.3">
@@ -21858,38 +21855,38 @@
       <c r="CM322" t="s">
         <v>403</v>
       </c>
-      <c r="CN322" t="s">
-        <v>404</v>
-      </c>
-      <c r="CO322" t="s">
-        <v>405</v>
-      </c>
-      <c r="CP322" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ322" t="s">
-        <v>407</v>
-      </c>
-      <c r="CR322" t="s">
-        <v>408</v>
-      </c>
-      <c r="CS322" t="s">
-        <v>409</v>
-      </c>
-      <c r="CT322" t="s">
-        <v>410</v>
-      </c>
-      <c r="CU322" t="s">
-        <v>411</v>
-      </c>
-      <c r="CV322" t="s">
-        <v>412</v>
-      </c>
-      <c r="CW322" t="s">
-        <v>413</v>
-      </c>
-      <c r="CX322" t="s">
-        <v>414</v>
+      <c r="CN322">
+        <v>0</v>
+      </c>
+      <c r="CO322">
+        <v>0</v>
+      </c>
+      <c r="CP322">
+        <v>0</v>
+      </c>
+      <c r="CQ322">
+        <v>0</v>
+      </c>
+      <c r="CR322">
+        <v>0</v>
+      </c>
+      <c r="CS322">
+        <v>0</v>
+      </c>
+      <c r="CT322">
+        <v>0</v>
+      </c>
+      <c r="CU322">
+        <v>0</v>
+      </c>
+      <c r="CV322">
+        <v>0</v>
+      </c>
+      <c r="CW322">
+        <v>0</v>
+      </c>
+      <c r="CX322">
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:106" x14ac:dyDescent="0.3">
@@ -21905,41 +21902,41 @@
       <c r="CM323" t="s">
         <v>403</v>
       </c>
-      <c r="CN323" t="s">
-        <v>404</v>
-      </c>
-      <c r="CO323" t="s">
-        <v>405</v>
-      </c>
-      <c r="CP323" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ323" t="s">
-        <v>407</v>
-      </c>
-      <c r="CR323" t="s">
-        <v>408</v>
-      </c>
-      <c r="CS323" t="s">
-        <v>409</v>
-      </c>
-      <c r="CT323" t="s">
-        <v>410</v>
-      </c>
-      <c r="CU323" t="s">
-        <v>411</v>
-      </c>
-      <c r="CV323" t="s">
-        <v>412</v>
-      </c>
-      <c r="CW323" t="s">
-        <v>413</v>
-      </c>
-      <c r="CX323" t="s">
-        <v>414</v>
-      </c>
-      <c r="CY323" t="s">
-        <v>415</v>
+      <c r="CN323">
+        <v>0</v>
+      </c>
+      <c r="CO323">
+        <v>0</v>
+      </c>
+      <c r="CP323">
+        <v>0</v>
+      </c>
+      <c r="CQ323">
+        <v>0</v>
+      </c>
+      <c r="CR323">
+        <v>0</v>
+      </c>
+      <c r="CS323">
+        <v>0</v>
+      </c>
+      <c r="CT323">
+        <v>0</v>
+      </c>
+      <c r="CU323">
+        <v>0</v>
+      </c>
+      <c r="CV323">
+        <v>0</v>
+      </c>
+      <c r="CW323">
+        <v>0</v>
+      </c>
+      <c r="CX323">
+        <v>0</v>
+      </c>
+      <c r="CY323">
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:106" x14ac:dyDescent="0.3">
@@ -21955,41 +21952,41 @@
       <c r="CM324" t="s">
         <v>403</v>
       </c>
-      <c r="CN324" t="s">
-        <v>404</v>
-      </c>
-      <c r="CO324" t="s">
-        <v>405</v>
-      </c>
-      <c r="CP324" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ324" t="s">
-        <v>407</v>
-      </c>
-      <c r="CR324" t="s">
-        <v>408</v>
-      </c>
-      <c r="CS324" t="s">
-        <v>409</v>
-      </c>
-      <c r="CT324" t="s">
-        <v>410</v>
-      </c>
-      <c r="CU324" t="s">
-        <v>411</v>
-      </c>
-      <c r="CV324" t="s">
-        <v>412</v>
-      </c>
-      <c r="CW324" t="s">
-        <v>413</v>
-      </c>
-      <c r="CX324" t="s">
-        <v>414</v>
-      </c>
-      <c r="CY324" t="s">
-        <v>415</v>
+      <c r="CN324">
+        <v>0</v>
+      </c>
+      <c r="CO324">
+        <v>0</v>
+      </c>
+      <c r="CP324">
+        <v>0</v>
+      </c>
+      <c r="CQ324">
+        <v>0</v>
+      </c>
+      <c r="CR324">
+        <v>0</v>
+      </c>
+      <c r="CS324">
+        <v>0</v>
+      </c>
+      <c r="CT324">
+        <v>0</v>
+      </c>
+      <c r="CU324">
+        <v>0</v>
+      </c>
+      <c r="CV324">
+        <v>0</v>
+      </c>
+      <c r="CW324">
+        <v>0</v>
+      </c>
+      <c r="CX324">
+        <v>0</v>
+      </c>
+      <c r="CY324">
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:106" x14ac:dyDescent="0.3">
@@ -22005,41 +22002,41 @@
       <c r="CM325" t="s">
         <v>403</v>
       </c>
-      <c r="CN325" t="s">
-        <v>404</v>
-      </c>
-      <c r="CO325" t="s">
-        <v>405</v>
-      </c>
-      <c r="CP325" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ325" t="s">
-        <v>407</v>
-      </c>
-      <c r="CR325" t="s">
-        <v>408</v>
-      </c>
-      <c r="CS325" t="s">
-        <v>409</v>
-      </c>
-      <c r="CT325" t="s">
-        <v>410</v>
-      </c>
-      <c r="CU325" t="s">
-        <v>411</v>
-      </c>
-      <c r="CV325" t="s">
-        <v>412</v>
-      </c>
-      <c r="CW325" t="s">
-        <v>413</v>
-      </c>
-      <c r="CX325" t="s">
-        <v>414</v>
-      </c>
-      <c r="CY325" t="s">
-        <v>415</v>
+      <c r="CN325">
+        <v>0</v>
+      </c>
+      <c r="CO325">
+        <v>0</v>
+      </c>
+      <c r="CP325">
+        <v>0</v>
+      </c>
+      <c r="CQ325">
+        <v>0</v>
+      </c>
+      <c r="CR325">
+        <v>0</v>
+      </c>
+      <c r="CS325">
+        <v>0</v>
+      </c>
+      <c r="CT325">
+        <v>0</v>
+      </c>
+      <c r="CU325">
+        <v>0</v>
+      </c>
+      <c r="CV325">
+        <v>0</v>
+      </c>
+      <c r="CW325">
+        <v>0</v>
+      </c>
+      <c r="CX325">
+        <v>0</v>
+      </c>
+      <c r="CY325">
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:106" x14ac:dyDescent="0.3">
@@ -22055,41 +22052,41 @@
       <c r="CM326" t="s">
         <v>403</v>
       </c>
-      <c r="CN326" t="s">
-        <v>404</v>
-      </c>
-      <c r="CO326" t="s">
-        <v>405</v>
-      </c>
-      <c r="CP326" t="s">
-        <v>406</v>
-      </c>
-      <c r="CQ326" t="s">
-        <v>407</v>
-      </c>
-      <c r="CR326" t="s">
-        <v>408</v>
-      </c>
-      <c r="CS326" t="s">
-        <v>409</v>
-      </c>
-      <c r="CT326" t="s">
-        <v>410</v>
-      </c>
-      <c r="CU326" t="s">
-        <v>411</v>
-      </c>
-      <c r="CV326" t="s">
-        <v>412</v>
-      </c>
-      <c r="CW326" t="s">
-        <v>413</v>
-      </c>
-      <c r="CX326" t="s">
-        <v>414</v>
-      </c>
-      <c r="CY326" t="s">
-        <v>415</v>
+      <c r="CN326">
+        <v>0</v>
+      </c>
+      <c r="CO326">
+        <v>0</v>
+      </c>
+      <c r="CP326">
+        <v>0</v>
+      </c>
+      <c r="CQ326">
+        <v>0</v>
+      </c>
+      <c r="CR326">
+        <v>0</v>
+      </c>
+      <c r="CS326">
+        <v>0</v>
+      </c>
+      <c r="CT326">
+        <v>0</v>
+      </c>
+      <c r="CU326">
+        <v>0</v>
+      </c>
+      <c r="CV326">
+        <v>0</v>
+      </c>
+      <c r="CW326">
+        <v>0</v>
+      </c>
+      <c r="CX326">
+        <v>0</v>
+      </c>
+      <c r="CY326">
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:106" x14ac:dyDescent="0.3">
@@ -22105,41 +22102,41 @@
       <c r="CM327" t="s">
         <v>402</v>
       </c>
-      <c r="CN327" t="s">
-        <v>403</v>
-      </c>
-      <c r="CO327" t="s">
-        <v>404</v>
-      </c>
-      <c r="CP327" t="s">
-        <v>405</v>
-      </c>
-      <c r="CQ327" t="s">
-        <v>406</v>
-      </c>
-      <c r="CR327" t="s">
-        <v>407</v>
-      </c>
-      <c r="CS327" t="s">
-        <v>408</v>
-      </c>
-      <c r="CT327" t="s">
-        <v>409</v>
-      </c>
-      <c r="CU327" t="s">
-        <v>410</v>
-      </c>
-      <c r="CV327" t="s">
-        <v>411</v>
-      </c>
-      <c r="CW327" t="s">
-        <v>412</v>
-      </c>
-      <c r="CX327" t="s">
-        <v>413</v>
-      </c>
-      <c r="CY327" t="s">
-        <v>414</v>
+      <c r="CN327">
+        <v>0</v>
+      </c>
+      <c r="CO327">
+        <v>0</v>
+      </c>
+      <c r="CP327">
+        <v>0</v>
+      </c>
+      <c r="CQ327">
+        <v>0</v>
+      </c>
+      <c r="CR327">
+        <v>0</v>
+      </c>
+      <c r="CS327">
+        <v>0</v>
+      </c>
+      <c r="CT327">
+        <v>0</v>
+      </c>
+      <c r="CU327">
+        <v>0</v>
+      </c>
+      <c r="CV327">
+        <v>0</v>
+      </c>
+      <c r="CW327">
+        <v>0</v>
+      </c>
+      <c r="CX327">
+        <v>0</v>
+      </c>
+      <c r="CY327">
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:106" x14ac:dyDescent="0.3">
@@ -22155,41 +22152,41 @@
       <c r="CM328" t="s">
         <v>402</v>
       </c>
-      <c r="CN328" t="s">
-        <v>403</v>
-      </c>
-      <c r="CO328" t="s">
-        <v>404</v>
-      </c>
-      <c r="CP328" t="s">
-        <v>405</v>
-      </c>
-      <c r="CQ328" t="s">
-        <v>406</v>
-      </c>
-      <c r="CR328" t="s">
-        <v>407</v>
-      </c>
-      <c r="CS328" t="s">
-        <v>408</v>
-      </c>
-      <c r="CT328" t="s">
-        <v>409</v>
-      </c>
-      <c r="CU328" t="s">
-        <v>410</v>
-      </c>
-      <c r="CV328" t="s">
-        <v>411</v>
-      </c>
-      <c r="CW328" t="s">
-        <v>412</v>
-      </c>
-      <c r="CX328" t="s">
-        <v>413</v>
-      </c>
-      <c r="CY328" t="s">
-        <v>414</v>
+      <c r="CN328">
+        <v>0</v>
+      </c>
+      <c r="CO328">
+        <v>0</v>
+      </c>
+      <c r="CP328">
+        <v>0</v>
+      </c>
+      <c r="CQ328">
+        <v>0</v>
+      </c>
+      <c r="CR328">
+        <v>0</v>
+      </c>
+      <c r="CS328">
+        <v>0</v>
+      </c>
+      <c r="CT328">
+        <v>0</v>
+      </c>
+      <c r="CU328">
+        <v>0</v>
+      </c>
+      <c r="CV328">
+        <v>0</v>
+      </c>
+      <c r="CW328">
+        <v>0</v>
+      </c>
+      <c r="CX328">
+        <v>0</v>
+      </c>
+      <c r="CY328">
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:106" x14ac:dyDescent="0.3">
@@ -53376,8 +53373,8 @@
       <c r="IU952" t="s">
         <v>414</v>
       </c>
-      <c r="IV952" t="s">
-        <v>415</v>
+      <c r="IV952">
+        <v>0</v>
       </c>
     </row>
     <row r="953" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53426,8 +53423,8 @@
       <c r="IU953" t="s">
         <v>413</v>
       </c>
-      <c r="IV953" t="s">
-        <v>414</v>
+      <c r="IV953">
+        <v>0</v>
       </c>
     </row>
     <row r="954" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53476,8 +53473,8 @@
       <c r="IU954" t="s">
         <v>413</v>
       </c>
-      <c r="IV954" t="s">
-        <v>414</v>
+      <c r="IV954">
+        <v>0</v>
       </c>
     </row>
     <row r="955" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53523,11 +53520,11 @@
       <c r="IU955" t="s">
         <v>413</v>
       </c>
-      <c r="IV955" t="s">
-        <v>414</v>
-      </c>
-      <c r="IW955" t="s">
-        <v>415</v>
+      <c r="IV955">
+        <v>0</v>
+      </c>
+      <c r="IW955">
+        <v>0</v>
       </c>
     </row>
     <row r="956" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53573,11 +53570,11 @@
       <c r="IU956" t="s">
         <v>413</v>
       </c>
-      <c r="IV956" t="s">
-        <v>414</v>
-      </c>
-      <c r="IW956" t="s">
-        <v>415</v>
+      <c r="IV956">
+        <v>0</v>
+      </c>
+      <c r="IW956">
+        <v>0</v>
       </c>
     </row>
     <row r="957" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53623,11 +53620,11 @@
       <c r="IU957" t="s">
         <v>412</v>
       </c>
-      <c r="IV957" t="s">
-        <v>413</v>
-      </c>
-      <c r="IW957" t="s">
-        <v>414</v>
+      <c r="IV957">
+        <v>0</v>
+      </c>
+      <c r="IW957">
+        <v>0</v>
       </c>
     </row>
     <row r="958" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53673,11 +53670,11 @@
       <c r="IU958" t="s">
         <v>412</v>
       </c>
-      <c r="IV958" t="s">
-        <v>413</v>
-      </c>
-      <c r="IW958" t="s">
-        <v>414</v>
+      <c r="IV958">
+        <v>0</v>
+      </c>
+      <c r="IW958">
+        <v>0</v>
       </c>
     </row>
     <row r="959" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53723,11 +53720,11 @@
       <c r="IU959" t="s">
         <v>412</v>
       </c>
-      <c r="IV959" t="s">
-        <v>413</v>
-      </c>
-      <c r="IW959" t="s">
-        <v>414</v>
+      <c r="IV959">
+        <v>0</v>
+      </c>
+      <c r="IW959">
+        <v>0</v>
       </c>
     </row>
     <row r="960" spans="1:258" hidden="1" x14ac:dyDescent="0.3">
@@ -53770,14 +53767,14 @@
       <c r="IU960" t="s">
         <v>412</v>
       </c>
-      <c r="IV960" t="s">
-        <v>413</v>
-      </c>
-      <c r="IW960" t="s">
-        <v>414</v>
-      </c>
-      <c r="IX960" t="s">
-        <v>415</v>
+      <c r="IV960">
+        <v>0</v>
+      </c>
+      <c r="IW960">
+        <v>0</v>
+      </c>
+      <c r="IX960">
+        <v>0</v>
       </c>
     </row>
     <row r="961" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -53820,14 +53817,14 @@
       <c r="IU961" t="s">
         <v>412</v>
       </c>
-      <c r="IV961" t="s">
-        <v>413</v>
-      </c>
-      <c r="IW961" t="s">
-        <v>414</v>
-      </c>
-      <c r="IX961" t="s">
-        <v>415</v>
+      <c r="IV961">
+        <v>0</v>
+      </c>
+      <c r="IW961">
+        <v>0</v>
+      </c>
+      <c r="IX961">
+        <v>0</v>
       </c>
     </row>
     <row r="962" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -53870,14 +53867,14 @@
       <c r="IU962" t="s">
         <v>411</v>
       </c>
-      <c r="IV962" t="s">
-        <v>412</v>
-      </c>
-      <c r="IW962" t="s">
-        <v>413</v>
-      </c>
-      <c r="IX962" t="s">
-        <v>414</v>
+      <c r="IV962">
+        <v>0</v>
+      </c>
+      <c r="IW962">
+        <v>0</v>
+      </c>
+      <c r="IX962">
+        <v>0</v>
       </c>
     </row>
     <row r="963" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -53920,14 +53917,14 @@
       <c r="IU963" t="s">
         <v>411</v>
       </c>
-      <c r="IV963" t="s">
-        <v>412</v>
-      </c>
-      <c r="IW963" t="s">
-        <v>413</v>
-      </c>
-      <c r="IX963" t="s">
-        <v>414</v>
+      <c r="IV963">
+        <v>0</v>
+      </c>
+      <c r="IW963">
+        <v>0</v>
+      </c>
+      <c r="IX963">
+        <v>0</v>
       </c>
     </row>
     <row r="964" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -53967,17 +53964,17 @@
       <c r="IU964" t="s">
         <v>411</v>
       </c>
-      <c r="IV964" t="s">
-        <v>412</v>
-      </c>
-      <c r="IW964" t="s">
-        <v>413</v>
-      </c>
-      <c r="IX964" t="s">
-        <v>414</v>
-      </c>
-      <c r="IY964" t="s">
-        <v>415</v>
+      <c r="IV964">
+        <v>0</v>
+      </c>
+      <c r="IW964">
+        <v>0</v>
+      </c>
+      <c r="IX964">
+        <v>0</v>
+      </c>
+      <c r="IY964">
+        <v>0</v>
       </c>
     </row>
     <row r="965" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54017,17 +54014,17 @@
       <c r="IU965" t="s">
         <v>411</v>
       </c>
-      <c r="IV965" t="s">
-        <v>412</v>
-      </c>
-      <c r="IW965" t="s">
-        <v>413</v>
-      </c>
-      <c r="IX965" t="s">
-        <v>414</v>
-      </c>
-      <c r="IY965" t="s">
-        <v>415</v>
+      <c r="IV965">
+        <v>0</v>
+      </c>
+      <c r="IW965">
+        <v>0</v>
+      </c>
+      <c r="IX965">
+        <v>0</v>
+      </c>
+      <c r="IY965">
+        <v>0</v>
       </c>
     </row>
     <row r="966" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54067,17 +54064,17 @@
       <c r="IU966" t="s">
         <v>410</v>
       </c>
-      <c r="IV966" t="s">
-        <v>411</v>
-      </c>
-      <c r="IW966" t="s">
-        <v>412</v>
-      </c>
-      <c r="IX966" t="s">
-        <v>413</v>
-      </c>
-      <c r="IY966" t="s">
-        <v>414</v>
+      <c r="IV966">
+        <v>0</v>
+      </c>
+      <c r="IW966">
+        <v>0</v>
+      </c>
+      <c r="IX966">
+        <v>0</v>
+      </c>
+      <c r="IY966">
+        <v>0</v>
       </c>
     </row>
     <row r="967" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54117,17 +54114,17 @@
       <c r="IU967" t="s">
         <v>410</v>
       </c>
-      <c r="IV967" t="s">
-        <v>411</v>
-      </c>
-      <c r="IW967" t="s">
-        <v>412</v>
-      </c>
-      <c r="IX967" t="s">
-        <v>413</v>
-      </c>
-      <c r="IY967" t="s">
-        <v>414</v>
+      <c r="IV967">
+        <v>0</v>
+      </c>
+      <c r="IW967">
+        <v>0</v>
+      </c>
+      <c r="IX967">
+        <v>0</v>
+      </c>
+      <c r="IY967">
+        <v>0</v>
       </c>
     </row>
     <row r="968" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54164,20 +54161,20 @@
       <c r="IU968" t="s">
         <v>410</v>
       </c>
-      <c r="IV968" t="s">
-        <v>411</v>
-      </c>
-      <c r="IW968" t="s">
-        <v>412</v>
-      </c>
-      <c r="IX968" t="s">
-        <v>413</v>
-      </c>
-      <c r="IY968" t="s">
-        <v>414</v>
-      </c>
-      <c r="IZ968" t="s">
-        <v>415</v>
+      <c r="IV968">
+        <v>0</v>
+      </c>
+      <c r="IW968">
+        <v>0</v>
+      </c>
+      <c r="IX968">
+        <v>0</v>
+      </c>
+      <c r="IY968">
+        <v>0</v>
+      </c>
+      <c r="IZ968">
+        <v>0</v>
       </c>
     </row>
     <row r="969" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54214,20 +54211,20 @@
       <c r="IU969" t="s">
         <v>410</v>
       </c>
-      <c r="IV969" t="s">
-        <v>411</v>
-      </c>
-      <c r="IW969" t="s">
-        <v>412</v>
-      </c>
-      <c r="IX969" t="s">
-        <v>413</v>
-      </c>
-      <c r="IY969" t="s">
-        <v>414</v>
-      </c>
-      <c r="IZ969" t="s">
-        <v>415</v>
+      <c r="IV969">
+        <v>0</v>
+      </c>
+      <c r="IW969">
+        <v>0</v>
+      </c>
+      <c r="IX969">
+        <v>0</v>
+      </c>
+      <c r="IY969">
+        <v>0</v>
+      </c>
+      <c r="IZ969">
+        <v>0</v>
       </c>
     </row>
     <row r="970" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54264,20 +54261,20 @@
       <c r="IU970" t="s">
         <v>409</v>
       </c>
-      <c r="IV970" t="s">
-        <v>410</v>
-      </c>
-      <c r="IW970" t="s">
-        <v>411</v>
-      </c>
-      <c r="IX970" t="s">
-        <v>412</v>
-      </c>
-      <c r="IY970" t="s">
-        <v>413</v>
-      </c>
-      <c r="IZ970" t="s">
-        <v>414</v>
+      <c r="IV970">
+        <v>0</v>
+      </c>
+      <c r="IW970">
+        <v>0</v>
+      </c>
+      <c r="IX970">
+        <v>0</v>
+      </c>
+      <c r="IY970">
+        <v>0</v>
+      </c>
+      <c r="IZ970">
+        <v>0</v>
       </c>
     </row>
     <row r="971" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54314,20 +54311,20 @@
       <c r="IU971" t="s">
         <v>409</v>
       </c>
-      <c r="IV971" t="s">
-        <v>410</v>
-      </c>
-      <c r="IW971" t="s">
-        <v>411</v>
-      </c>
-      <c r="IX971" t="s">
-        <v>412</v>
-      </c>
-      <c r="IY971" t="s">
-        <v>413</v>
-      </c>
-      <c r="IZ971" t="s">
-        <v>414</v>
+      <c r="IV971">
+        <v>0</v>
+      </c>
+      <c r="IW971">
+        <v>0</v>
+      </c>
+      <c r="IX971">
+        <v>0</v>
+      </c>
+      <c r="IY971">
+        <v>0</v>
+      </c>
+      <c r="IZ971">
+        <v>0</v>
       </c>
     </row>
     <row r="972" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54361,23 +54358,23 @@
       <c r="IU972" t="s">
         <v>409</v>
       </c>
-      <c r="IV972" t="s">
-        <v>410</v>
-      </c>
-      <c r="IW972" t="s">
-        <v>411</v>
-      </c>
-      <c r="IX972" t="s">
-        <v>412</v>
-      </c>
-      <c r="IY972" t="s">
-        <v>413</v>
-      </c>
-      <c r="IZ972" t="s">
-        <v>414</v>
-      </c>
-      <c r="JA972" t="s">
-        <v>415</v>
+      <c r="IV972">
+        <v>0</v>
+      </c>
+      <c r="IW972">
+        <v>0</v>
+      </c>
+      <c r="IX972">
+        <v>0</v>
+      </c>
+      <c r="IY972">
+        <v>0</v>
+      </c>
+      <c r="IZ972">
+        <v>0</v>
+      </c>
+      <c r="JA972">
+        <v>0</v>
       </c>
     </row>
     <row r="973" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54411,23 +54408,23 @@
       <c r="IU973" t="s">
         <v>409</v>
       </c>
-      <c r="IV973" t="s">
-        <v>410</v>
-      </c>
-      <c r="IW973" t="s">
-        <v>411</v>
-      </c>
-      <c r="IX973" t="s">
-        <v>412</v>
-      </c>
-      <c r="IY973" t="s">
-        <v>413</v>
-      </c>
-      <c r="IZ973" t="s">
-        <v>414</v>
-      </c>
-      <c r="JA973" t="s">
-        <v>415</v>
+      <c r="IV973">
+        <v>0</v>
+      </c>
+      <c r="IW973">
+        <v>0</v>
+      </c>
+      <c r="IX973">
+        <v>0</v>
+      </c>
+      <c r="IY973">
+        <v>0</v>
+      </c>
+      <c r="IZ973">
+        <v>0</v>
+      </c>
+      <c r="JA973">
+        <v>0</v>
       </c>
     </row>
     <row r="974" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54461,23 +54458,23 @@
       <c r="IU974" t="s">
         <v>408</v>
       </c>
-      <c r="IV974" t="s">
-        <v>409</v>
-      </c>
-      <c r="IW974" t="s">
-        <v>410</v>
-      </c>
-      <c r="IX974" t="s">
-        <v>411</v>
-      </c>
-      <c r="IY974" t="s">
-        <v>412</v>
-      </c>
-      <c r="IZ974" t="s">
-        <v>413</v>
-      </c>
-      <c r="JA974" t="s">
-        <v>414</v>
+      <c r="IV974">
+        <v>0</v>
+      </c>
+      <c r="IW974">
+        <v>0</v>
+      </c>
+      <c r="IX974">
+        <v>0</v>
+      </c>
+      <c r="IY974">
+        <v>0</v>
+      </c>
+      <c r="IZ974">
+        <v>0</v>
+      </c>
+      <c r="JA974">
+        <v>0</v>
       </c>
     </row>
     <row r="975" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54511,23 +54508,23 @@
       <c r="IU975" t="s">
         <v>408</v>
       </c>
-      <c r="IV975" t="s">
-        <v>409</v>
-      </c>
-      <c r="IW975" t="s">
-        <v>410</v>
-      </c>
-      <c r="IX975" t="s">
-        <v>411</v>
-      </c>
-      <c r="IY975" t="s">
-        <v>412</v>
-      </c>
-      <c r="IZ975" t="s">
-        <v>413</v>
-      </c>
-      <c r="JA975" t="s">
-        <v>414</v>
+      <c r="IV975">
+        <v>0</v>
+      </c>
+      <c r="IW975">
+        <v>0</v>
+      </c>
+      <c r="IX975">
+        <v>0</v>
+      </c>
+      <c r="IY975">
+        <v>0</v>
+      </c>
+      <c r="IZ975">
+        <v>0</v>
+      </c>
+      <c r="JA975">
+        <v>0</v>
       </c>
     </row>
     <row r="976" spans="1:262" hidden="1" x14ac:dyDescent="0.3">
@@ -54558,26 +54555,26 @@
       <c r="IU976" t="s">
         <v>408</v>
       </c>
-      <c r="IV976" t="s">
-        <v>409</v>
-      </c>
-      <c r="IW976" t="s">
-        <v>410</v>
-      </c>
-      <c r="IX976" t="s">
-        <v>411</v>
-      </c>
-      <c r="IY976" t="s">
-        <v>412</v>
-      </c>
-      <c r="IZ976" t="s">
-        <v>413</v>
-      </c>
-      <c r="JA976" t="s">
-        <v>414</v>
-      </c>
-      <c r="JB976" t="s">
-        <v>415</v>
+      <c r="IV976">
+        <v>0</v>
+      </c>
+      <c r="IW976">
+        <v>0</v>
+      </c>
+      <c r="IX976">
+        <v>0</v>
+      </c>
+      <c r="IY976">
+        <v>0</v>
+      </c>
+      <c r="IZ976">
+        <v>0</v>
+      </c>
+      <c r="JA976">
+        <v>0</v>
+      </c>
+      <c r="JB976">
+        <v>0</v>
       </c>
     </row>
     <row r="977" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54608,26 +54605,26 @@
       <c r="IU977" t="s">
         <v>408</v>
       </c>
-      <c r="IV977" t="s">
-        <v>409</v>
-      </c>
-      <c r="IW977" t="s">
-        <v>410</v>
-      </c>
-      <c r="IX977" t="s">
-        <v>411</v>
-      </c>
-      <c r="IY977" t="s">
-        <v>412</v>
-      </c>
-      <c r="IZ977" t="s">
-        <v>413</v>
-      </c>
-      <c r="JA977" t="s">
-        <v>414</v>
-      </c>
-      <c r="JB977" t="s">
-        <v>415</v>
+      <c r="IV977">
+        <v>0</v>
+      </c>
+      <c r="IW977">
+        <v>0</v>
+      </c>
+      <c r="IX977">
+        <v>0</v>
+      </c>
+      <c r="IY977">
+        <v>0</v>
+      </c>
+      <c r="IZ977">
+        <v>0</v>
+      </c>
+      <c r="JA977">
+        <v>0</v>
+      </c>
+      <c r="JB977">
+        <v>0</v>
       </c>
     </row>
     <row r="978" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54658,26 +54655,26 @@
       <c r="IU978" t="s">
         <v>407</v>
       </c>
-      <c r="IV978" t="s">
-        <v>408</v>
-      </c>
-      <c r="IW978" t="s">
-        <v>409</v>
-      </c>
-      <c r="IX978" t="s">
-        <v>410</v>
-      </c>
-      <c r="IY978" t="s">
-        <v>411</v>
-      </c>
-      <c r="IZ978" t="s">
-        <v>412</v>
-      </c>
-      <c r="JA978" t="s">
-        <v>413</v>
-      </c>
-      <c r="JB978" t="s">
-        <v>414</v>
+      <c r="IV978">
+        <v>0</v>
+      </c>
+      <c r="IW978">
+        <v>0</v>
+      </c>
+      <c r="IX978">
+        <v>0</v>
+      </c>
+      <c r="IY978">
+        <v>0</v>
+      </c>
+      <c r="IZ978">
+        <v>0</v>
+      </c>
+      <c r="JA978">
+        <v>0</v>
+      </c>
+      <c r="JB978">
+        <v>0</v>
       </c>
     </row>
     <row r="979" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54708,26 +54705,26 @@
       <c r="IU979" t="s">
         <v>407</v>
       </c>
-      <c r="IV979" t="s">
-        <v>408</v>
-      </c>
-      <c r="IW979" t="s">
-        <v>409</v>
-      </c>
-      <c r="IX979" t="s">
-        <v>410</v>
-      </c>
-      <c r="IY979" t="s">
-        <v>411</v>
-      </c>
-      <c r="IZ979" t="s">
-        <v>412</v>
-      </c>
-      <c r="JA979" t="s">
-        <v>413</v>
-      </c>
-      <c r="JB979" t="s">
-        <v>414</v>
+      <c r="IV979">
+        <v>0</v>
+      </c>
+      <c r="IW979">
+        <v>0</v>
+      </c>
+      <c r="IX979">
+        <v>0</v>
+      </c>
+      <c r="IY979">
+        <v>0</v>
+      </c>
+      <c r="IZ979">
+        <v>0</v>
+      </c>
+      <c r="JA979">
+        <v>0</v>
+      </c>
+      <c r="JB979">
+        <v>0</v>
       </c>
     </row>
     <row r="980" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54755,29 +54752,29 @@
       <c r="IU980" t="s">
         <v>407</v>
       </c>
-      <c r="IV980" t="s">
-        <v>408</v>
-      </c>
-      <c r="IW980" t="s">
-        <v>409</v>
-      </c>
-      <c r="IX980" t="s">
-        <v>410</v>
-      </c>
-      <c r="IY980" t="s">
-        <v>411</v>
-      </c>
-      <c r="IZ980" t="s">
-        <v>412</v>
-      </c>
-      <c r="JA980" t="s">
-        <v>413</v>
-      </c>
-      <c r="JB980" t="s">
-        <v>414</v>
-      </c>
-      <c r="JC980" t="s">
-        <v>415</v>
+      <c r="IV980">
+        <v>0</v>
+      </c>
+      <c r="IW980">
+        <v>0</v>
+      </c>
+      <c r="IX980">
+        <v>0</v>
+      </c>
+      <c r="IY980">
+        <v>0</v>
+      </c>
+      <c r="IZ980">
+        <v>0</v>
+      </c>
+      <c r="JA980">
+        <v>0</v>
+      </c>
+      <c r="JB980">
+        <v>0</v>
+      </c>
+      <c r="JC980">
+        <v>0</v>
       </c>
     </row>
     <row r="981" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54805,29 +54802,29 @@
       <c r="IU981" t="s">
         <v>407</v>
       </c>
-      <c r="IV981" t="s">
-        <v>408</v>
-      </c>
-      <c r="IW981" t="s">
-        <v>409</v>
-      </c>
-      <c r="IX981" t="s">
-        <v>410</v>
-      </c>
-      <c r="IY981" t="s">
-        <v>411</v>
-      </c>
-      <c r="IZ981" t="s">
-        <v>412</v>
-      </c>
-      <c r="JA981" t="s">
-        <v>413</v>
-      </c>
-      <c r="JB981" t="s">
-        <v>414</v>
-      </c>
-      <c r="JC981" t="s">
-        <v>415</v>
+      <c r="IV981">
+        <v>0</v>
+      </c>
+      <c r="IW981">
+        <v>0</v>
+      </c>
+      <c r="IX981">
+        <v>0</v>
+      </c>
+      <c r="IY981">
+        <v>0</v>
+      </c>
+      <c r="IZ981">
+        <v>0</v>
+      </c>
+      <c r="JA981">
+        <v>0</v>
+      </c>
+      <c r="JB981">
+        <v>0</v>
+      </c>
+      <c r="JC981">
+        <v>0</v>
       </c>
     </row>
     <row r="982" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54855,29 +54852,29 @@
       <c r="IU982" t="s">
         <v>407</v>
       </c>
-      <c r="IV982" t="s">
-        <v>408</v>
-      </c>
-      <c r="IW982" t="s">
-        <v>409</v>
-      </c>
-      <c r="IX982" t="s">
-        <v>410</v>
-      </c>
-      <c r="IY982" t="s">
-        <v>411</v>
-      </c>
-      <c r="IZ982" t="s">
-        <v>412</v>
-      </c>
-      <c r="JA982" t="s">
-        <v>413</v>
-      </c>
-      <c r="JB982" t="s">
-        <v>414</v>
-      </c>
-      <c r="JC982" t="s">
-        <v>415</v>
+      <c r="IV982">
+        <v>0</v>
+      </c>
+      <c r="IW982">
+        <v>0</v>
+      </c>
+      <c r="IX982">
+        <v>0</v>
+      </c>
+      <c r="IY982">
+        <v>0</v>
+      </c>
+      <c r="IZ982">
+        <v>0</v>
+      </c>
+      <c r="JA982">
+        <v>0</v>
+      </c>
+      <c r="JB982">
+        <v>0</v>
+      </c>
+      <c r="JC982">
+        <v>0</v>
       </c>
     </row>
     <row r="983" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54905,29 +54902,29 @@
       <c r="IU983" t="s">
         <v>406</v>
       </c>
-      <c r="IV983" t="s">
-        <v>407</v>
-      </c>
-      <c r="IW983" t="s">
-        <v>408</v>
-      </c>
-      <c r="IX983" t="s">
-        <v>409</v>
-      </c>
-      <c r="IY983" t="s">
-        <v>410</v>
-      </c>
-      <c r="IZ983" t="s">
-        <v>411</v>
-      </c>
-      <c r="JA983" t="s">
-        <v>412</v>
-      </c>
-      <c r="JB983" t="s">
-        <v>413</v>
-      </c>
-      <c r="JC983" t="s">
-        <v>414</v>
+      <c r="IV983">
+        <v>0</v>
+      </c>
+      <c r="IW983">
+        <v>0</v>
+      </c>
+      <c r="IX983">
+        <v>0</v>
+      </c>
+      <c r="IY983">
+        <v>0</v>
+      </c>
+      <c r="IZ983">
+        <v>0</v>
+      </c>
+      <c r="JA983">
+        <v>0</v>
+      </c>
+      <c r="JB983">
+        <v>0</v>
+      </c>
+      <c r="JC983">
+        <v>0</v>
       </c>
     </row>
     <row r="984" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -54955,29 +54952,29 @@
       <c r="IU984" t="s">
         <v>406</v>
       </c>
-      <c r="IV984" t="s">
-        <v>407</v>
-      </c>
-      <c r="IW984" t="s">
-        <v>408</v>
-      </c>
-      <c r="IX984" t="s">
-        <v>409</v>
-      </c>
-      <c r="IY984" t="s">
-        <v>410</v>
-      </c>
-      <c r="IZ984" t="s">
-        <v>411</v>
-      </c>
-      <c r="JA984" t="s">
-        <v>412</v>
-      </c>
-      <c r="JB984" t="s">
-        <v>413</v>
-      </c>
-      <c r="JC984" t="s">
-        <v>414</v>
+      <c r="IV984">
+        <v>0</v>
+      </c>
+      <c r="IW984">
+        <v>0</v>
+      </c>
+      <c r="IX984">
+        <v>0</v>
+      </c>
+      <c r="IY984">
+        <v>0</v>
+      </c>
+      <c r="IZ984">
+        <v>0</v>
+      </c>
+      <c r="JA984">
+        <v>0</v>
+      </c>
+      <c r="JB984">
+        <v>0</v>
+      </c>
+      <c r="JC984">
+        <v>0</v>
       </c>
     </row>
     <row r="985" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55002,32 +54999,32 @@
       <c r="IU985" t="s">
         <v>406</v>
       </c>
-      <c r="IV985" t="s">
-        <v>407</v>
-      </c>
-      <c r="IW985" t="s">
-        <v>408</v>
-      </c>
-      <c r="IX985" t="s">
-        <v>409</v>
-      </c>
-      <c r="IY985" t="s">
-        <v>410</v>
-      </c>
-      <c r="IZ985" t="s">
-        <v>411</v>
-      </c>
-      <c r="JA985" t="s">
-        <v>412</v>
-      </c>
-      <c r="JB985" t="s">
-        <v>413</v>
-      </c>
-      <c r="JC985" t="s">
-        <v>414</v>
-      </c>
-      <c r="JD985" t="s">
-        <v>415</v>
+      <c r="IV985">
+        <v>0</v>
+      </c>
+      <c r="IW985">
+        <v>0</v>
+      </c>
+      <c r="IX985">
+        <v>0</v>
+      </c>
+      <c r="IY985">
+        <v>0</v>
+      </c>
+      <c r="IZ985">
+        <v>0</v>
+      </c>
+      <c r="JA985">
+        <v>0</v>
+      </c>
+      <c r="JB985">
+        <v>0</v>
+      </c>
+      <c r="JC985">
+        <v>0</v>
+      </c>
+      <c r="JD985">
+        <v>0</v>
       </c>
     </row>
     <row r="986" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55052,32 +55049,32 @@
       <c r="IU986" t="s">
         <v>406</v>
       </c>
-      <c r="IV986" t="s">
-        <v>407</v>
-      </c>
-      <c r="IW986" t="s">
-        <v>408</v>
-      </c>
-      <c r="IX986" t="s">
-        <v>409</v>
-      </c>
-      <c r="IY986" t="s">
-        <v>410</v>
-      </c>
-      <c r="IZ986" t="s">
-        <v>411</v>
-      </c>
-      <c r="JA986" t="s">
-        <v>412</v>
-      </c>
-      <c r="JB986" t="s">
-        <v>413</v>
-      </c>
-      <c r="JC986" t="s">
-        <v>414</v>
-      </c>
-      <c r="JD986" t="s">
-        <v>415</v>
+      <c r="IV986">
+        <v>0</v>
+      </c>
+      <c r="IW986">
+        <v>0</v>
+      </c>
+      <c r="IX986">
+        <v>0</v>
+      </c>
+      <c r="IY986">
+        <v>0</v>
+      </c>
+      <c r="IZ986">
+        <v>0</v>
+      </c>
+      <c r="JA986">
+        <v>0</v>
+      </c>
+      <c r="JB986">
+        <v>0</v>
+      </c>
+      <c r="JC986">
+        <v>0</v>
+      </c>
+      <c r="JD986">
+        <v>0</v>
       </c>
     </row>
     <row r="987" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55102,32 +55099,32 @@
       <c r="IU987" t="s">
         <v>405</v>
       </c>
-      <c r="IV987" t="s">
-        <v>406</v>
-      </c>
-      <c r="IW987" t="s">
-        <v>407</v>
-      </c>
-      <c r="IX987" t="s">
-        <v>408</v>
-      </c>
-      <c r="IY987" t="s">
-        <v>409</v>
-      </c>
-      <c r="IZ987" t="s">
-        <v>410</v>
-      </c>
-      <c r="JA987" t="s">
-        <v>411</v>
-      </c>
-      <c r="JB987" t="s">
-        <v>412</v>
-      </c>
-      <c r="JC987" t="s">
-        <v>413</v>
-      </c>
-      <c r="JD987" t="s">
-        <v>414</v>
+      <c r="IV987">
+        <v>0</v>
+      </c>
+      <c r="IW987">
+        <v>0</v>
+      </c>
+      <c r="IX987">
+        <v>0</v>
+      </c>
+      <c r="IY987">
+        <v>0</v>
+      </c>
+      <c r="IZ987">
+        <v>0</v>
+      </c>
+      <c r="JA987">
+        <v>0</v>
+      </c>
+      <c r="JB987">
+        <v>0</v>
+      </c>
+      <c r="JC987">
+        <v>0</v>
+      </c>
+      <c r="JD987">
+        <v>0</v>
       </c>
     </row>
     <row r="988" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55152,32 +55149,32 @@
       <c r="IU988" t="s">
         <v>405</v>
       </c>
-      <c r="IV988" t="s">
-        <v>406</v>
-      </c>
-      <c r="IW988" t="s">
-        <v>407</v>
-      </c>
-      <c r="IX988" t="s">
-        <v>408</v>
-      </c>
-      <c r="IY988" t="s">
-        <v>409</v>
-      </c>
-      <c r="IZ988" t="s">
-        <v>410</v>
-      </c>
-      <c r="JA988" t="s">
-        <v>411</v>
-      </c>
-      <c r="JB988" t="s">
-        <v>412</v>
-      </c>
-      <c r="JC988" t="s">
-        <v>413</v>
-      </c>
-      <c r="JD988" t="s">
-        <v>414</v>
+      <c r="IV988">
+        <v>0</v>
+      </c>
+      <c r="IW988">
+        <v>0</v>
+      </c>
+      <c r="IX988">
+        <v>0</v>
+      </c>
+      <c r="IY988">
+        <v>0</v>
+      </c>
+      <c r="IZ988">
+        <v>0</v>
+      </c>
+      <c r="JA988">
+        <v>0</v>
+      </c>
+      <c r="JB988">
+        <v>0</v>
+      </c>
+      <c r="JC988">
+        <v>0</v>
+      </c>
+      <c r="JD988">
+        <v>0</v>
       </c>
     </row>
     <row r="989" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55199,35 +55196,35 @@
       <c r="IU989" t="s">
         <v>405</v>
       </c>
-      <c r="IV989" t="s">
-        <v>406</v>
-      </c>
-      <c r="IW989" t="s">
-        <v>407</v>
-      </c>
-      <c r="IX989" t="s">
-        <v>408</v>
-      </c>
-      <c r="IY989" t="s">
-        <v>409</v>
-      </c>
-      <c r="IZ989" t="s">
-        <v>410</v>
-      </c>
-      <c r="JA989" t="s">
-        <v>411</v>
-      </c>
-      <c r="JB989" t="s">
-        <v>412</v>
-      </c>
-      <c r="JC989" t="s">
-        <v>413</v>
-      </c>
-      <c r="JD989" t="s">
-        <v>414</v>
-      </c>
-      <c r="JE989" t="s">
-        <v>415</v>
+      <c r="IV989">
+        <v>0</v>
+      </c>
+      <c r="IW989">
+        <v>0</v>
+      </c>
+      <c r="IX989">
+        <v>0</v>
+      </c>
+      <c r="IY989">
+        <v>0</v>
+      </c>
+      <c r="IZ989">
+        <v>0</v>
+      </c>
+      <c r="JA989">
+        <v>0</v>
+      </c>
+      <c r="JB989">
+        <v>0</v>
+      </c>
+      <c r="JC989">
+        <v>0</v>
+      </c>
+      <c r="JD989">
+        <v>0</v>
+      </c>
+      <c r="JE989">
+        <v>0</v>
       </c>
     </row>
     <row r="990" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55249,35 +55246,35 @@
       <c r="IU990" t="s">
         <v>405</v>
       </c>
-      <c r="IV990" t="s">
-        <v>406</v>
-      </c>
-      <c r="IW990" t="s">
-        <v>407</v>
-      </c>
-      <c r="IX990" t="s">
-        <v>408</v>
-      </c>
-      <c r="IY990" t="s">
-        <v>409</v>
-      </c>
-      <c r="IZ990" t="s">
-        <v>410</v>
-      </c>
-      <c r="JA990" t="s">
-        <v>411</v>
-      </c>
-      <c r="JB990" t="s">
-        <v>412</v>
-      </c>
-      <c r="JC990" t="s">
-        <v>413</v>
-      </c>
-      <c r="JD990" t="s">
-        <v>414</v>
-      </c>
-      <c r="JE990" t="s">
-        <v>415</v>
+      <c r="IV990">
+        <v>0</v>
+      </c>
+      <c r="IW990">
+        <v>0</v>
+      </c>
+      <c r="IX990">
+        <v>0</v>
+      </c>
+      <c r="IY990">
+        <v>0</v>
+      </c>
+      <c r="IZ990">
+        <v>0</v>
+      </c>
+      <c r="JA990">
+        <v>0</v>
+      </c>
+      <c r="JB990">
+        <v>0</v>
+      </c>
+      <c r="JC990">
+        <v>0</v>
+      </c>
+      <c r="JD990">
+        <v>0</v>
+      </c>
+      <c r="JE990">
+        <v>0</v>
       </c>
     </row>
     <row r="991" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55299,35 +55296,35 @@
       <c r="IU991" t="s">
         <v>404</v>
       </c>
-      <c r="IV991" t="s">
-        <v>405</v>
-      </c>
-      <c r="IW991" t="s">
-        <v>406</v>
-      </c>
-      <c r="IX991" t="s">
-        <v>407</v>
-      </c>
-      <c r="IY991" t="s">
-        <v>408</v>
-      </c>
-      <c r="IZ991" t="s">
-        <v>409</v>
-      </c>
-      <c r="JA991" t="s">
-        <v>410</v>
-      </c>
-      <c r="JB991" t="s">
-        <v>411</v>
-      </c>
-      <c r="JC991" t="s">
-        <v>412</v>
-      </c>
-      <c r="JD991" t="s">
-        <v>413</v>
-      </c>
-      <c r="JE991" t="s">
-        <v>414</v>
+      <c r="IV991">
+        <v>0</v>
+      </c>
+      <c r="IW991">
+        <v>0</v>
+      </c>
+      <c r="IX991">
+        <v>0</v>
+      </c>
+      <c r="IY991">
+        <v>0</v>
+      </c>
+      <c r="IZ991">
+        <v>0</v>
+      </c>
+      <c r="JA991">
+        <v>0</v>
+      </c>
+      <c r="JB991">
+        <v>0</v>
+      </c>
+      <c r="JC991">
+        <v>0</v>
+      </c>
+      <c r="JD991">
+        <v>0</v>
+      </c>
+      <c r="JE991">
+        <v>0</v>
       </c>
     </row>
     <row r="992" spans="1:265" hidden="1" x14ac:dyDescent="0.3">
@@ -55349,35 +55346,35 @@
       <c r="IU992" t="s">
         <v>404</v>
       </c>
-      <c r="IV992" t="s">
-        <v>405</v>
-      </c>
-      <c r="IW992" t="s">
-        <v>406</v>
-      </c>
-      <c r="IX992" t="s">
-        <v>407</v>
-      </c>
-      <c r="IY992" t="s">
-        <v>408</v>
-      </c>
-      <c r="IZ992" t="s">
-        <v>409</v>
-      </c>
-      <c r="JA992" t="s">
-        <v>410</v>
-      </c>
-      <c r="JB992" t="s">
-        <v>411</v>
-      </c>
-      <c r="JC992" t="s">
-        <v>412</v>
-      </c>
-      <c r="JD992" t="s">
-        <v>413</v>
-      </c>
-      <c r="JE992" t="s">
-        <v>414</v>
+      <c r="IV992">
+        <v>0</v>
+      </c>
+      <c r="IW992">
+        <v>0</v>
+      </c>
+      <c r="IX992">
+        <v>0</v>
+      </c>
+      <c r="IY992">
+        <v>0</v>
+      </c>
+      <c r="IZ992">
+        <v>0</v>
+      </c>
+      <c r="JA992">
+        <v>0</v>
+      </c>
+      <c r="JB992">
+        <v>0</v>
+      </c>
+      <c r="JC992">
+        <v>0</v>
+      </c>
+      <c r="JD992">
+        <v>0</v>
+      </c>
+      <c r="JE992">
+        <v>0</v>
       </c>
     </row>
     <row r="993" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55396,38 +55393,38 @@
       <c r="IU993" t="s">
         <v>404</v>
       </c>
-      <c r="IV993" t="s">
-        <v>405</v>
-      </c>
-      <c r="IW993" t="s">
-        <v>406</v>
-      </c>
-      <c r="IX993" t="s">
-        <v>407</v>
-      </c>
-      <c r="IY993" t="s">
-        <v>408</v>
-      </c>
-      <c r="IZ993" t="s">
-        <v>409</v>
-      </c>
-      <c r="JA993" t="s">
-        <v>410</v>
-      </c>
-      <c r="JB993" t="s">
-        <v>411</v>
-      </c>
-      <c r="JC993" t="s">
-        <v>412</v>
-      </c>
-      <c r="JD993" t="s">
-        <v>413</v>
-      </c>
-      <c r="JE993" t="s">
-        <v>414</v>
-      </c>
-      <c r="JF993" t="s">
-        <v>415</v>
+      <c r="IV993">
+        <v>0</v>
+      </c>
+      <c r="IW993">
+        <v>0</v>
+      </c>
+      <c r="IX993">
+        <v>0</v>
+      </c>
+      <c r="IY993">
+        <v>0</v>
+      </c>
+      <c r="IZ993">
+        <v>0</v>
+      </c>
+      <c r="JA993">
+        <v>0</v>
+      </c>
+      <c r="JB993">
+        <v>0</v>
+      </c>
+      <c r="JC993">
+        <v>0</v>
+      </c>
+      <c r="JD993">
+        <v>0</v>
+      </c>
+      <c r="JE993">
+        <v>0</v>
+      </c>
+      <c r="JF993">
+        <v>0</v>
       </c>
     </row>
     <row r="994" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55446,38 +55443,38 @@
       <c r="IU994" t="s">
         <v>404</v>
       </c>
-      <c r="IV994" t="s">
-        <v>405</v>
-      </c>
-      <c r="IW994" t="s">
-        <v>406</v>
-      </c>
-      <c r="IX994" t="s">
-        <v>407</v>
-      </c>
-      <c r="IY994" t="s">
-        <v>408</v>
-      </c>
-      <c r="IZ994" t="s">
-        <v>409</v>
-      </c>
-      <c r="JA994" t="s">
-        <v>410</v>
-      </c>
-      <c r="JB994" t="s">
-        <v>411</v>
-      </c>
-      <c r="JC994" t="s">
-        <v>412</v>
-      </c>
-      <c r="JD994" t="s">
-        <v>413</v>
-      </c>
-      <c r="JE994" t="s">
-        <v>414</v>
-      </c>
-      <c r="JF994" t="s">
-        <v>415</v>
+      <c r="IV994">
+        <v>0</v>
+      </c>
+      <c r="IW994">
+        <v>0</v>
+      </c>
+      <c r="IX994">
+        <v>0</v>
+      </c>
+      <c r="IY994">
+        <v>0</v>
+      </c>
+      <c r="IZ994">
+        <v>0</v>
+      </c>
+      <c r="JA994">
+        <v>0</v>
+      </c>
+      <c r="JB994">
+        <v>0</v>
+      </c>
+      <c r="JC994">
+        <v>0</v>
+      </c>
+      <c r="JD994">
+        <v>0</v>
+      </c>
+      <c r="JE994">
+        <v>0</v>
+      </c>
+      <c r="JF994">
+        <v>0</v>
       </c>
     </row>
     <row r="995" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55496,38 +55493,38 @@
       <c r="IU995" t="s">
         <v>403</v>
       </c>
-      <c r="IV995" t="s">
-        <v>404</v>
-      </c>
-      <c r="IW995" t="s">
-        <v>405</v>
-      </c>
-      <c r="IX995" t="s">
-        <v>406</v>
-      </c>
-      <c r="IY995" t="s">
-        <v>407</v>
-      </c>
-      <c r="IZ995" t="s">
-        <v>408</v>
-      </c>
-      <c r="JA995" t="s">
-        <v>409</v>
-      </c>
-      <c r="JB995" t="s">
-        <v>410</v>
-      </c>
-      <c r="JC995" t="s">
-        <v>411</v>
-      </c>
-      <c r="JD995" t="s">
-        <v>412</v>
-      </c>
-      <c r="JE995" t="s">
-        <v>413</v>
-      </c>
-      <c r="JF995" t="s">
-        <v>414</v>
+      <c r="IV995">
+        <v>0</v>
+      </c>
+      <c r="IW995">
+        <v>0</v>
+      </c>
+      <c r="IX995">
+        <v>0</v>
+      </c>
+      <c r="IY995">
+        <v>0</v>
+      </c>
+      <c r="IZ995">
+        <v>0</v>
+      </c>
+      <c r="JA995">
+        <v>0</v>
+      </c>
+      <c r="JB995">
+        <v>0</v>
+      </c>
+      <c r="JC995">
+        <v>0</v>
+      </c>
+      <c r="JD995">
+        <v>0</v>
+      </c>
+      <c r="JE995">
+        <v>0</v>
+      </c>
+      <c r="JF995">
+        <v>0</v>
       </c>
     </row>
     <row r="996" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55546,38 +55543,38 @@
       <c r="IU996" t="s">
         <v>403</v>
       </c>
-      <c r="IV996" t="s">
-        <v>404</v>
-      </c>
-      <c r="IW996" t="s">
-        <v>405</v>
-      </c>
-      <c r="IX996" t="s">
-        <v>406</v>
-      </c>
-      <c r="IY996" t="s">
-        <v>407</v>
-      </c>
-      <c r="IZ996" t="s">
-        <v>408</v>
-      </c>
-      <c r="JA996" t="s">
-        <v>409</v>
-      </c>
-      <c r="JB996" t="s">
-        <v>410</v>
-      </c>
-      <c r="JC996" t="s">
-        <v>411</v>
-      </c>
-      <c r="JD996" t="s">
-        <v>412</v>
-      </c>
-      <c r="JE996" t="s">
-        <v>413</v>
-      </c>
-      <c r="JF996" t="s">
-        <v>414</v>
+      <c r="IV996">
+        <v>0</v>
+      </c>
+      <c r="IW996">
+        <v>0</v>
+      </c>
+      <c r="IX996">
+        <v>0</v>
+      </c>
+      <c r="IY996">
+        <v>0</v>
+      </c>
+      <c r="IZ996">
+        <v>0</v>
+      </c>
+      <c r="JA996">
+        <v>0</v>
+      </c>
+      <c r="JB996">
+        <v>0</v>
+      </c>
+      <c r="JC996">
+        <v>0</v>
+      </c>
+      <c r="JD996">
+        <v>0</v>
+      </c>
+      <c r="JE996">
+        <v>0</v>
+      </c>
+      <c r="JF996">
+        <v>0</v>
       </c>
     </row>
     <row r="997" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55593,41 +55590,41 @@
       <c r="IU997" t="s">
         <v>403</v>
       </c>
-      <c r="IV997" t="s">
-        <v>404</v>
-      </c>
-      <c r="IW997" t="s">
-        <v>405</v>
-      </c>
-      <c r="IX997" t="s">
-        <v>406</v>
-      </c>
-      <c r="IY997" t="s">
-        <v>407</v>
-      </c>
-      <c r="IZ997" t="s">
-        <v>408</v>
-      </c>
-      <c r="JA997" t="s">
-        <v>409</v>
-      </c>
-      <c r="JB997" t="s">
-        <v>410</v>
-      </c>
-      <c r="JC997" t="s">
-        <v>411</v>
-      </c>
-      <c r="JD997" t="s">
-        <v>412</v>
-      </c>
-      <c r="JE997" t="s">
-        <v>413</v>
-      </c>
-      <c r="JF997" t="s">
-        <v>414</v>
-      </c>
-      <c r="JG997" t="s">
-        <v>415</v>
+      <c r="IV997">
+        <v>0</v>
+      </c>
+      <c r="IW997">
+        <v>0</v>
+      </c>
+      <c r="IX997">
+        <v>0</v>
+      </c>
+      <c r="IY997">
+        <v>0</v>
+      </c>
+      <c r="IZ997">
+        <v>0</v>
+      </c>
+      <c r="JA997">
+        <v>0</v>
+      </c>
+      <c r="JB997">
+        <v>0</v>
+      </c>
+      <c r="JC997">
+        <v>0</v>
+      </c>
+      <c r="JD997">
+        <v>0</v>
+      </c>
+      <c r="JE997">
+        <v>0</v>
+      </c>
+      <c r="JF997">
+        <v>0</v>
+      </c>
+      <c r="JG997">
+        <v>0</v>
       </c>
     </row>
     <row r="998" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55643,41 +55640,41 @@
       <c r="IU998" t="s">
         <v>403</v>
       </c>
-      <c r="IV998" t="s">
-        <v>404</v>
-      </c>
-      <c r="IW998" t="s">
-        <v>405</v>
-      </c>
-      <c r="IX998" t="s">
-        <v>406</v>
-      </c>
-      <c r="IY998" t="s">
-        <v>407</v>
-      </c>
-      <c r="IZ998" t="s">
-        <v>408</v>
-      </c>
-      <c r="JA998" t="s">
-        <v>409</v>
-      </c>
-      <c r="JB998" t="s">
-        <v>410</v>
-      </c>
-      <c r="JC998" t="s">
-        <v>411</v>
-      </c>
-      <c r="JD998" t="s">
-        <v>412</v>
-      </c>
-      <c r="JE998" t="s">
-        <v>413</v>
-      </c>
-      <c r="JF998" t="s">
-        <v>414</v>
-      </c>
-      <c r="JG998" t="s">
-        <v>415</v>
+      <c r="IV998">
+        <v>0</v>
+      </c>
+      <c r="IW998">
+        <v>0</v>
+      </c>
+      <c r="IX998">
+        <v>0</v>
+      </c>
+      <c r="IY998">
+        <v>0</v>
+      </c>
+      <c r="IZ998">
+        <v>0</v>
+      </c>
+      <c r="JA998">
+        <v>0</v>
+      </c>
+      <c r="JB998">
+        <v>0</v>
+      </c>
+      <c r="JC998">
+        <v>0</v>
+      </c>
+      <c r="JD998">
+        <v>0</v>
+      </c>
+      <c r="JE998">
+        <v>0</v>
+      </c>
+      <c r="JF998">
+        <v>0</v>
+      </c>
+      <c r="JG998">
+        <v>0</v>
       </c>
     </row>
     <row r="999" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55693,41 +55690,41 @@
       <c r="IU999" t="s">
         <v>402</v>
       </c>
-      <c r="IV999" t="s">
-        <v>403</v>
-      </c>
-      <c r="IW999" t="s">
-        <v>404</v>
-      </c>
-      <c r="IX999" t="s">
-        <v>405</v>
-      </c>
-      <c r="IY999" t="s">
-        <v>406</v>
-      </c>
-      <c r="IZ999" t="s">
-        <v>407</v>
-      </c>
-      <c r="JA999" t="s">
-        <v>408</v>
-      </c>
-      <c r="JB999" t="s">
-        <v>409</v>
-      </c>
-      <c r="JC999" t="s">
-        <v>410</v>
-      </c>
-      <c r="JD999" t="s">
-        <v>411</v>
-      </c>
-      <c r="JE999" t="s">
-        <v>412</v>
-      </c>
-      <c r="JF999" t="s">
-        <v>413</v>
-      </c>
-      <c r="JG999" t="s">
-        <v>414</v>
+      <c r="IV999">
+        <v>0</v>
+      </c>
+      <c r="IW999">
+        <v>0</v>
+      </c>
+      <c r="IX999">
+        <v>0</v>
+      </c>
+      <c r="IY999">
+        <v>0</v>
+      </c>
+      <c r="IZ999">
+        <v>0</v>
+      </c>
+      <c r="JA999">
+        <v>0</v>
+      </c>
+      <c r="JB999">
+        <v>0</v>
+      </c>
+      <c r="JC999">
+        <v>0</v>
+      </c>
+      <c r="JD999">
+        <v>0</v>
+      </c>
+      <c r="JE999">
+        <v>0</v>
+      </c>
+      <c r="JF999">
+        <v>0</v>
+      </c>
+      <c r="JG999">
+        <v>0</v>
       </c>
     </row>
     <row r="1000" spans="1:269" hidden="1" x14ac:dyDescent="0.3">
@@ -55743,41 +55740,41 @@
       <c r="IU1000" t="s">
         <v>402</v>
       </c>
-      <c r="IV1000" t="s">
-        <v>403</v>
-      </c>
-      <c r="IW1000" t="s">
-        <v>404</v>
-      </c>
-      <c r="IX1000" t="s">
-        <v>405</v>
-      </c>
-      <c r="IY1000" t="s">
-        <v>406</v>
-      </c>
-      <c r="IZ1000" t="s">
-        <v>407</v>
-      </c>
-      <c r="JA1000" t="s">
-        <v>408</v>
-      </c>
-      <c r="JB1000" t="s">
-        <v>409</v>
-      </c>
-      <c r="JC1000" t="s">
-        <v>410</v>
-      </c>
-      <c r="JD1000" t="s">
-        <v>411</v>
-      </c>
-      <c r="JE1000" t="s">
-        <v>412</v>
-      </c>
-      <c r="JF1000" t="s">
-        <v>413</v>
-      </c>
-      <c r="JG1000" t="s">
-        <v>414</v>
+      <c r="IV1000">
+        <v>0</v>
+      </c>
+      <c r="IW1000">
+        <v>0</v>
+      </c>
+      <c r="IX1000">
+        <v>0</v>
+      </c>
+      <c r="IY1000">
+        <v>0</v>
+      </c>
+      <c r="IZ1000">
+        <v>0</v>
+      </c>
+      <c r="JA1000">
+        <v>0</v>
+      </c>
+      <c r="JB1000">
+        <v>0</v>
+      </c>
+      <c r="JC1000">
+        <v>0</v>
+      </c>
+      <c r="JD1000">
+        <v>0</v>
+      </c>
+      <c r="JE1000">
+        <v>0</v>
+      </c>
+      <c r="JF1000">
+        <v>0</v>
+      </c>
+      <c r="JG1000">
+        <v>0</v>
       </c>
     </row>
     <row r="1001" spans="1:269" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>